<commit_message>
Fix ReadMe + Excel
</commit_message>
<xml_diff>
--- a/Declaração de imposto/Puma Plan.xlsx
+++ b/Declaração de imposto/Puma Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvnc0\Downloads\Projeto-Excel\Declaração de imposto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871B8090-1A36-4A25-929D-8292F04F5F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A89B91C-C739-48C0-BB56-B9B180D57805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13704" yWindow="1140" windowWidth="9336" windowHeight="11100" tabRatio="0" firstSheet="2" activeTab="2" xr2:uid="{1C1F6274-6663-434E-B6B1-2886BA4432A3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="0" firstSheet="2" activeTab="2" xr2:uid="{1C1F6274-6663-434E-B6B1-2886BA4432A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Informes" sheetId="15" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="92">
   <si>
     <t xml:space="preserve"> Banco do Brasil</t>
   </si>
@@ -291,9 +291,6 @@
   </si>
   <si>
     <t>2. DADOS DO TÍTULAR</t>
-  </si>
-  <si>
-    <t>abril-2025</t>
   </si>
   <si>
     <t>xxxxxxx@email.com</t>
@@ -336,7 +333,7 @@
     <numFmt numFmtId="168" formatCode="&quot;(&quot;00&quot;) &quot;00000&quot;-&quot;0000"/>
     <numFmt numFmtId="169" formatCode="&quot;0000000000&quot;"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -479,6 +476,14 @@
       <color theme="0"/>
       <name val="Segoe UI Light"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="13">
@@ -640,13 +645,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -790,8 +796,13 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="168" fontId="20" fillId="7" borderId="2" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="Hiperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Neutro" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3114,13 +3125,13 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2743200</xdr:colOff>
+      <xdr:colOff>2674620</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>106680</xdr:colOff>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>110490</xdr:rowOff>
     </xdr:to>
@@ -3208,7 +3219,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1409700</xdr:colOff>
+      <xdr:colOff>1341120</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>102870</xdr:rowOff>
     </xdr:to>
@@ -3610,7 +3621,7 @@
   <dimension ref="A2:G25"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="C14" sqref="C14:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3646,7 +3657,7 @@
     <row r="6" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C6" s="19">
         <f>SUM(D10,D15,D20)</f>
-        <v>13200500</v>
+        <v>1023500</v>
       </c>
       <c r="D6" s="19"/>
     </row>
@@ -3662,7 +3673,7 @@
         <v>70</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G9" s="3"/>
     </row>
@@ -3672,7 +3683,7 @@
         <v>71</v>
       </c>
       <c r="D10" s="8">
-        <v>12300000</v>
+        <v>123000</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="16.8" x14ac:dyDescent="0.4">
@@ -3681,7 +3692,7 @@
         <v>72</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
@@ -3720,7 +3731,7 @@
         <v>72</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
@@ -3760,7 +3771,7 @@
         <v>72</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
@@ -3805,7 +3816,7 @@
   <dimension ref="A2:H25"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3835,7 +3846,7 @@
         <v>51</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="16.8" x14ac:dyDescent="0.4">
@@ -3851,7 +3862,7 @@
         <v>53</v>
       </c>
       <c r="D7" s="38">
-        <v>22730</v>
+        <v>24556</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="16.8" x14ac:dyDescent="0.4">
@@ -3860,7 +3871,7 @@
         <v>54</v>
       </c>
       <c r="D8" s="42">
-        <v>0</v>
+        <v>555555555555555</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="16.8" x14ac:dyDescent="0.4">
@@ -3869,7 +3880,7 @@
         <v>55</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H9" s="3"/>
     </row>
@@ -3879,7 +3890,7 @@
         <v>56</v>
       </c>
       <c r="D10" s="36" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="16.8" x14ac:dyDescent="0.4">
@@ -3888,7 +3899,7 @@
         <v>57</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="16.8" x14ac:dyDescent="0.4">
@@ -3897,7 +3908,7 @@
         <v>58</v>
       </c>
       <c r="D12" s="39" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="16.8" x14ac:dyDescent="0.4">
@@ -3923,8 +3934,8 @@
       <c r="C15" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="41" t="s">
-        <v>84</v>
+      <c r="D15" s="50" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="16.8" x14ac:dyDescent="0.4">
@@ -3983,6 +3994,7 @@
       <c r="C25" s="3"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="3">
     <mergeCell ref="A1:A1048576"/>
     <mergeCell ref="C3:D3"/>
@@ -4007,13 +4019,13 @@
   <dimension ref="A2:G37"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="40.6640625" style="44" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.88671875" customWidth="1"/>
@@ -4055,8 +4067,8 @@
       <c r="F6" s="12"/>
     </row>
     <row r="7" spans="2:7" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C7" s="23" t="s">
-        <v>83</v>
+      <c r="C7" s="23">
+        <v>45748</v>
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="25">
@@ -4701,6 +4713,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="851b35d3-0456-4d6a-bc2f-da927e91d158">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="19483571-f922-4e8e-9c1c-26f0a2252132" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010001E48B58A68BE64E9120D347E3E06B3A" ma:contentTypeVersion="19" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="2f90046ec77328b7f86417d2e03b3d33">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="851b35d3-0456-4d6a-bc2f-da927e91d158" xmlns:ns3="19483571-f922-4e8e-9c1c-26f0a2252132" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c815006ac2d4f05ee97fdd57e40d8e38" ns2:_="" ns3:_="">
     <xsd:import namespace="851b35d3-0456-4d6a-bc2f-da927e91d158"/>
@@ -4955,27 +4987,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9680C06D-F603-4315-BF13-982EB8576E3A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="851b35d3-0456-4d6a-bc2f-da927e91d158"/>
+    <ds:schemaRef ds:uri="19483571-f922-4e8e-9c1c-26f0a2252132"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="851b35d3-0456-4d6a-bc2f-da927e91d158">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="19483571-f922-4e8e-9c1c-26f0a2252132" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B69849B-37F1-4594-8DF9-7938EC83CA4F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D98F71B4-0C4E-464B-8DD1-FE385FAE2FB1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4992,23 +5023,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B69849B-37F1-4594-8DF9-7938EC83CA4F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9680C06D-F603-4315-BF13-982EB8576E3A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="851b35d3-0456-4d6a-bc2f-da927e91d158"/>
-    <ds:schemaRef ds:uri="19483571-f922-4e8e-9c1c-26f0a2252132"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>